<commit_message>
El ultimo commit de la batalla final
</commit_message>
<xml_diff>
--- a/Proyecto final pruebas.xlsx
+++ b/Proyecto final pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProjectProgrammer\Python\Trabajos practicos\ProyectoFinal\ProyectoFinal23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12BC9A98-FE49-4328-BAB7-E4FA2D4AE8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481B5930-D9B8-4BA7-8075-487E14751C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCD56C2B-7EFC-4439-B006-08DEE2259B23}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Nombre del Proyecto</t>
   </si>
@@ -85,14 +85,47 @@
     <t>Buenos Aires, Argentina</t>
   </si>
   <si>
-    <t xml:space="preserve">Proyecto Final Coder House Python (Comisión </t>
+    <t>Proyecto Final CODERHOUSE PYTHON (Comision: 47770)</t>
+  </si>
+  <si>
+    <t>Lucas Gak</t>
+  </si>
+  <si>
+    <t>Opera</t>
+  </si>
+  <si>
+    <t>103.0.4928.34</t>
+  </si>
+  <si>
+    <t>SMART TRAINING (Academia de deportes)</t>
+  </si>
+  <si>
+    <t>Registro de usuario</t>
+  </si>
+  <si>
+    <t>Registra tu usuario y te pide logearte con el mismo</t>
+  </si>
+  <si>
+    <t>Funcion de los links de la navbar</t>
+  </si>
+  <si>
+    <t>Te dirige a distintas secciones de la pagina</t>
+  </si>
+  <si>
+    <t>Dirigirte a distintas secciones de la pagina</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Te desloguea de tu cuenta y te ofrece volver a loguear o volver al inicio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +135,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -157,6 +198,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -476,16 +520,16 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -500,7 +544,9 @@
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -514,26 +560,34 @@
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="6"/>
       <c r="D4" s="1" t="s">
         <v>10</v>
@@ -567,10 +621,18 @@
       <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="B7" s="4">
+        <v>45220</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
@@ -579,22 +641,38 @@
       <c r="A8" s="3">
         <v>2</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="4">
+        <v>45220</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="4">
+        <v>45220</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="F9" s="3" t="s">
         <v>14</v>
       </c>

</xml_diff>